<commit_message>
Update Dynamic Filtering (Filter,Unique).xlsx
</commit_message>
<xml_diff>
--- a/VBA & Excel/VBA/Archive/Dynamic Filtering (Filter,Unique).xlsx
+++ b/VBA & Excel/VBA/Archive/Dynamic Filtering (Filter,Unique).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\9. 내 드롭박스\@. #오빠두\@ 엑셀 - 영상강의\1c_엑셀 전문가 강의\엑셀함수강의\고급강의 filter 함수 사용법 실전예제 총정리\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Languages\VBA &amp; Excel\VBA\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8B74C8-9077-40F5-89E9-987035968713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B98F4-EC1C-4DE0-B4F5-AC0586DD76D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{302F6E57-047A-4A08-98A7-610E6095B446}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{302F6E57-047A-4A08-98A7-610E6095B446}"/>
   </bookViews>
   <sheets>
     <sheet name="FILTER함수-예제" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -509,7 +509,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>날짜</t>
+    <t>월</t>
   </si>
 </sst>
 </file>
@@ -1418,322 +1418,322 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="106"/>
                 <c:pt idx="0">
-                  <c:v>517000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>756000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>239200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>324000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1355700</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>618300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>522100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>281600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1058000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>225000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>869500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>340000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>411900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>568600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1042000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>397700</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>446500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>76800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>258000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>247900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1496000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>336000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>179400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>184800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>160000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>318200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1314800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>590900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>71400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>234300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>547200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>358800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>360000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>437000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>361900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>460000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>251800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>180000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>549100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>211200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>633400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>273000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>737300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>106600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>847900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>381300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>411100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>412000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>220900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>344000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>138600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>38400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>395300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>488600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1119300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>608900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1969600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1015100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>562700</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>388000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>224200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>434300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>331800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>406000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>442200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>200600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>235600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>496400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>313200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>189000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>94600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>637400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>827600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>831900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>503700</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>430200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>176700</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>327600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>724400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>566100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>326600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>347100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>406200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1368100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1226500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>122500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>94300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>284700</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>338400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>475600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>184000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1143400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>775600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>684900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>349600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>327600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>332500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>713600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>619200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>319600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>704900</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>798400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>75000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2119,322 +2119,322 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="106"/>
                 <c:pt idx="0">
-                  <c:v>155</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>168</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>320</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>64</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>282</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>230</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>87</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>107</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>130</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>281</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>86</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>67</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>395</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>96</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>56</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>74</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>328</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>133</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>71</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>152</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>92</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>81</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>102</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>77</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>64</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>48</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>165</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>91</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>177</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>26</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>223</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>87</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>87</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>47</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>86</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>106</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>116</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>275</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>143</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>480</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>280</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>129</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>97</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>101</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>79</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>121</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>122</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>58</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>76</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>106</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>87</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>54</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>166</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>225</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>211</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>148</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>116</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>57</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>84</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>162</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>153</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>71</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>89</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>103</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>355</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>302</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>73</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>72</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>136</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>275</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>183</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>184</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>92</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>84</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>169</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>141</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>68</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>176</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>226</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3594,32 +3594,32 @@
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.69921875" customWidth="1"/>
-    <col min="2" max="2" width="10.796875" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" customWidth="1"/>
-    <col min="4" max="4" width="9.8984375" style="26" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="11.25" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="32" t="s">
         <v>133</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="33"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="34" t="s">
         <v>134</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" s="27" t="s">
         <v>0</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" s="29" t="s">
         <v>129</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" s="8" t="s">
         <v>131</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
         <v>129</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="s">
         <v>130</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="s">
         <v>131</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>131</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
         <v>130</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>132</v>
       </c>
@@ -3768,30 +3768,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E048D6E-8879-403D-90DB-C4E9F1E814F5}">
   <dimension ref="A2:AD233"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18.75" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.296875" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="10.8984375" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="31.3984375" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.19921875" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.8984375" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="3.25" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="31.375" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.875" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="10" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="12.8984375" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="3.09765625" customWidth="1"/>
-    <col min="9" max="9" width="12.69921875" style="21" customWidth="1"/>
-    <col min="10" max="10" width="36.59765625" customWidth="1"/>
-    <col min="11" max="11" width="8.796875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.69921875" customWidth="1"/>
-    <col min="13" max="13" width="8.796875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="5.09765625" customWidth="1"/>
-    <col min="16" max="16" width="12.19921875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="3.125" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="21" customWidth="1"/>
+    <col min="10" max="10" width="36.625" customWidth="1"/>
+    <col min="11" max="11" width="8.75" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1"/>
+    <col min="13" max="13" width="8.75" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="5.125" customWidth="1"/>
+    <col min="16" max="16" width="12.25" style="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="18" width="13" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="30" width="8.796875" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="30" width="8.75" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
@@ -3819,7 +3821,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B3" s="4">
         <v>43831</v>
       </c>
@@ -3841,13 +3843,12 @@
       <c r="I3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="7">
         <v>43831</v>
       </c>
@@ -3867,7 +3868,7 @@
         <v>262800</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="7">
         <v>43832</v>
       </c>
@@ -3914,7 +3915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>43833</v>
       </c>
@@ -3934,7 +3935,13 @@
         <v>364500</v>
       </c>
       <c r="I6" s="24" cm="1">
-        <f t="array" ref="I6:N233">_xlfn._xlws.FILTER(tbl판매내역[],IF(J2="",tbl판매내역[날짜]=tbl판매내역[날짜],IF(L2="월",MONTH(tbl판매내역[날짜])=J2,IF(L2="날짜",tbl판매내역[날짜]=J2,WEEKDAY(tbl판매내역[날짜])=J2)))*IF(J3="",tbl판매내역[제품명]=tbl판매내역[제품명],IF(L3="정확히일치",tbl판매내역[제품명]=J3,ISNUMBER(SEARCH(J3,tbl판매내역[제품명])))),"결과 없음")</f>
+        <f t="array" ref="I6:N233">_xlfn._xlws.FILTER(tbl판매내역[],
+IF(J2="",tbl판매내역[날짜]=tbl판매내역[날짜],
+IF(L2="월",MONTH(tbl판매내역[날짜])=J2,
+IF(L2="날짜",tbl판매내역[날짜]=J2,WEEKDAY(tbl판매내역[날짜])=J2)))
+*IF(J3="",tbl판매내역[제품명]=tbl판매내역[제품명],
+IF(L3="정확히일치",tbl판매내역[제품명]=J3,
+ISNUMBER(SEARCH(J3,tbl판매내역[제품명])))),"결과 없음")</f>
         <v>43831</v>
       </c>
       <c r="J6" t="str">
@@ -3958,14 +3965,14 @@
       </c>
       <c r="Q6" s="16">
         <f ca="1">SUMIF(I:I,P6,L:L)</f>
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="R6" s="16">
         <f ca="1">SUMIF(I:I,P6,N:N)</f>
-        <v>517000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>43833</v>
       </c>
@@ -4008,14 +4015,14 @@
       </c>
       <c r="Q7" s="16">
         <f t="shared" ref="Q7:Q15" ca="1" si="0">SUMIF(I:I,P7,L:L)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R7" s="16">
         <f t="shared" ref="R7:R15" ca="1" si="1">SUMIF(I:I,P7,N:N)</f>
-        <v>54400</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>43834</v>
       </c>
@@ -4058,14 +4065,14 @@
       </c>
       <c r="Q8" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>756000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B9" s="7">
         <v>43835</v>
       </c>
@@ -4108,14 +4115,14 @@
       </c>
       <c r="Q9" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="R9" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>239200</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <v>43836</v>
       </c>
@@ -4158,14 +4165,14 @@
       </c>
       <c r="Q10" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="R10" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>324000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B11" s="7">
         <v>43837</v>
       </c>
@@ -4208,14 +4215,14 @@
       </c>
       <c r="Q11" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="R11" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>105300</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B12" s="7">
         <v>43837</v>
       </c>
@@ -4258,14 +4265,14 @@
       </c>
       <c r="Q12" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="R12" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>1355700</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B13" s="7">
         <v>43837</v>
       </c>
@@ -4308,14 +4315,14 @@
       </c>
       <c r="Q13" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="R13" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>618300</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B14" s="7">
         <v>43837</v>
       </c>
@@ -4358,14 +4365,14 @@
       </c>
       <c r="Q14" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="R14" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>522100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B15" s="7">
         <v>43837</v>
       </c>
@@ -4408,14 +4415,14 @@
       </c>
       <c r="Q15" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="R15" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>281600</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B16" s="7">
         <v>43837</v>
       </c>
@@ -4458,14 +4465,14 @@
       </c>
       <c r="Q16" s="16">
         <f t="shared" ref="Q16:Q17" ca="1" si="2">SUMIF(I:I,P16,L:L)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="R16" s="16">
         <f t="shared" ref="R16:R17" ca="1" si="3">SUMIF(I:I,P16,N:N)</f>
-        <v>52800</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B17" s="7">
         <v>43837</v>
       </c>
@@ -4508,14 +4515,14 @@
       </c>
       <c r="Q17" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>282</v>
+        <v>0</v>
       </c>
       <c r="R17" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>1058000</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B18" s="7">
         <v>43838</v>
       </c>
@@ -4558,14 +4565,14 @@
       </c>
       <c r="Q18" s="16">
         <f t="shared" ref="Q18:Q29" ca="1" si="4">SUMIF(I:I,P18,L:L)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="R18" s="16">
         <f t="shared" ref="R18:R29" ca="1" si="5">SUMIF(I:I,P18,N:N)</f>
-        <v>225000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B19" s="7">
         <v>43838</v>
       </c>
@@ -4608,14 +4615,14 @@
       </c>
       <c r="Q19" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="R19" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>869500</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B20" s="7">
         <v>43838</v>
       </c>
@@ -4658,14 +4665,14 @@
       </c>
       <c r="Q20" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="R20" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>340000</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B21" s="7">
         <v>43839</v>
       </c>
@@ -4708,14 +4715,14 @@
       </c>
       <c r="Q21" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="R21" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>411900</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B22" s="7">
         <v>43839</v>
       </c>
@@ -4758,14 +4765,14 @@
       </c>
       <c r="Q22" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="R22" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>568600</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B23" s="7">
         <v>43840</v>
       </c>
@@ -4808,14 +4815,14 @@
       </c>
       <c r="Q23" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>281</v>
+        <v>0</v>
       </c>
       <c r="R23" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>1042000</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B24" s="7">
         <v>43840</v>
       </c>
@@ -4858,14 +4865,14 @@
       </c>
       <c r="Q24" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="R24" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>397700</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B25" s="7">
         <v>43841</v>
       </c>
@@ -4908,14 +4915,14 @@
       </c>
       <c r="Q25" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="R25" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>446500</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B26" s="7">
         <v>43842</v>
       </c>
@@ -4958,14 +4965,14 @@
       </c>
       <c r="Q26" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="R26" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>76800</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B27" s="7">
         <v>43842</v>
       </c>
@@ -5008,14 +5015,14 @@
       </c>
       <c r="Q27" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="R27" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>258000</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B28" s="7">
         <v>43842</v>
       </c>
@@ -5058,14 +5065,14 @@
       </c>
       <c r="Q28" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="R28" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>247900</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B29" s="7">
         <v>43842</v>
       </c>
@@ -5108,14 +5115,14 @@
       </c>
       <c r="Q29" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>395</v>
+        <v>0</v>
       </c>
       <c r="R29" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>1496000</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B30" s="7">
         <v>43842</v>
       </c>
@@ -5158,14 +5165,14 @@
       </c>
       <c r="Q30" s="16">
         <f t="shared" ref="Q30:Q93" ca="1" si="6">SUMIF(I:I,P30,L:L)</f>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="R30" s="16">
         <f t="shared" ref="R30:R93" ca="1" si="7">SUMIF(I:I,P30,N:N)</f>
-        <v>336000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B31" s="7">
         <v>43843</v>
       </c>
@@ -5208,14 +5215,14 @@
       </c>
       <c r="Q31" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="R31" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>179400</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B32" s="7">
         <v>43844</v>
       </c>
@@ -5258,14 +5265,14 @@
       </c>
       <c r="Q32" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="R32" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>184800</v>
-      </c>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B33" s="7">
         <v>43844</v>
       </c>
@@ -5308,14 +5315,14 @@
       </c>
       <c r="Q33" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="R33" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>160000</v>
-      </c>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B34" s="7">
         <v>43844</v>
       </c>
@@ -5358,14 +5365,14 @@
       </c>
       <c r="Q34" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="R34" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>318200</v>
-      </c>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B35" s="7">
         <v>43844</v>
       </c>
@@ -5408,14 +5415,14 @@
       </c>
       <c r="Q35" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>328</v>
+        <v>0</v>
       </c>
       <c r="R35" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>1314800</v>
-      </c>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B36" s="7">
         <v>43844</v>
       </c>
@@ -5458,14 +5465,14 @@
       </c>
       <c r="Q36" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="R36" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>590900</v>
-      </c>
-    </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B37" s="7">
         <v>43844</v>
       </c>
@@ -5508,14 +5515,14 @@
       </c>
       <c r="Q37" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="R37" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>71400</v>
-      </c>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B38" s="7">
         <v>43844</v>
       </c>
@@ -5558,14 +5565,14 @@
       </c>
       <c r="Q38" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="R38" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>234300</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B39" s="7">
         <v>43844</v>
       </c>
@@ -5608,14 +5615,14 @@
       </c>
       <c r="Q39" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="R39" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>547200</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B40" s="7">
         <v>43844</v>
       </c>
@@ -5658,14 +5665,14 @@
       </c>
       <c r="Q40" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="R40" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>358800</v>
-      </c>
-    </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B41" s="7">
         <v>43845</v>
       </c>
@@ -5708,14 +5715,14 @@
       </c>
       <c r="Q41" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="R41" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>360000</v>
-      </c>
-    </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B42" s="7">
         <v>43845</v>
       </c>
@@ -5758,14 +5765,14 @@
       </c>
       <c r="Q42" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="R42" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>437000</v>
-      </c>
-    </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B43" s="7">
         <v>43846</v>
       </c>
@@ -5808,14 +5815,14 @@
       </c>
       <c r="Q43" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="R43" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>361900</v>
-      </c>
-    </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B44" s="7">
         <v>43846</v>
       </c>
@@ -5858,14 +5865,14 @@
       </c>
       <c r="Q44" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R44" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>460000</v>
-      </c>
-    </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B45" s="7">
         <v>43847</v>
       </c>
@@ -5908,14 +5915,14 @@
       </c>
       <c r="Q45" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="R45" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>251800</v>
-      </c>
-    </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B46" s="7">
         <v>43847</v>
       </c>
@@ -5958,14 +5965,14 @@
       </c>
       <c r="Q46" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="R46" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>180000</v>
-      </c>
-    </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B47" s="7">
         <v>43848</v>
       </c>
@@ -6008,14 +6015,14 @@
       </c>
       <c r="Q47" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="R47" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>549100</v>
-      </c>
-    </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B48" s="7">
         <v>43848</v>
       </c>
@@ -6058,14 +6065,14 @@
       </c>
       <c r="Q48" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="R48" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>211200</v>
-      </c>
-    </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B49" s="7">
         <v>43848</v>
       </c>
@@ -6108,14 +6115,14 @@
       </c>
       <c r="Q49" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="R49" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>633400</v>
-      </c>
-    </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B50" s="7">
         <v>43848</v>
       </c>
@@ -6158,14 +6165,14 @@
       </c>
       <c r="Q50" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="R50" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>273000</v>
-      </c>
-    </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B51" s="7">
         <v>43848</v>
       </c>
@@ -6208,14 +6215,14 @@
       </c>
       <c r="Q51" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="R51" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>737300</v>
-      </c>
-    </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B52" s="7">
         <v>43849</v>
       </c>
@@ -6258,14 +6265,14 @@
       </c>
       <c r="Q52" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="R52" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>106600</v>
-      </c>
-    </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B53" s="7">
         <v>43849</v>
       </c>
@@ -6308,14 +6315,14 @@
       </c>
       <c r="Q53" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>223</v>
+        <v>0</v>
       </c>
       <c r="R53" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>847900</v>
-      </c>
-    </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B54" s="7">
         <v>43850</v>
       </c>
@@ -6358,14 +6365,14 @@
       </c>
       <c r="Q54" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="R54" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>381300</v>
-      </c>
-    </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B55" s="7">
         <v>43851</v>
       </c>
@@ -6408,14 +6415,14 @@
       </c>
       <c r="Q55" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="R55" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>411100</v>
-      </c>
-    </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B56" s="7">
         <v>43852</v>
       </c>
@@ -6458,14 +6465,14 @@
       </c>
       <c r="Q56" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R56" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>412000</v>
-      </c>
-    </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B57" s="7">
         <v>43853</v>
       </c>
@@ -6508,14 +6515,14 @@
       </c>
       <c r="Q57" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="R57" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>220900</v>
-      </c>
-    </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B58" s="7">
         <v>43854</v>
       </c>
@@ -6558,14 +6565,14 @@
       </c>
       <c r="Q58" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="R58" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>344000</v>
-      </c>
-    </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B59" s="7">
         <v>43854</v>
       </c>
@@ -6608,14 +6615,14 @@
       </c>
       <c r="Q59" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="R59" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>138600</v>
-      </c>
-    </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B60" s="7">
         <v>43854</v>
       </c>
@@ -6658,14 +6665,14 @@
       </c>
       <c r="Q60" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="R60" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>38400</v>
-      </c>
-    </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B61" s="7">
         <v>43854</v>
       </c>
@@ -6708,14 +6715,14 @@
       </c>
       <c r="Q61" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="R61" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>395300</v>
-      </c>
-    </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B62" s="7">
         <v>43854</v>
       </c>
@@ -6758,14 +6765,14 @@
       </c>
       <c r="Q62" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="R62" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>488600</v>
-      </c>
-    </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B63" s="7">
         <v>43854</v>
       </c>
@@ -6808,14 +6815,14 @@
       </c>
       <c r="Q63" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>275</v>
+        <v>0</v>
       </c>
       <c r="R63" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>1119300</v>
-      </c>
-    </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B64" s="7">
         <v>43854</v>
       </c>
@@ -6858,14 +6865,14 @@
       </c>
       <c r="Q64" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="R64" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>608900</v>
-      </c>
-    </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B65" s="7">
         <v>43855</v>
       </c>
@@ -6908,14 +6915,14 @@
       </c>
       <c r="Q65" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="R65" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>1969600</v>
-      </c>
-    </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B66" s="7">
         <v>43856</v>
       </c>
@@ -6958,14 +6965,14 @@
       </c>
       <c r="Q66" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="R66" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>1015100</v>
-      </c>
-    </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B67" s="7">
         <v>43857</v>
       </c>
@@ -7008,14 +7015,14 @@
       </c>
       <c r="Q67" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="R67" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>562700</v>
-      </c>
-    </row>
-    <row r="68" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B68" s="7">
         <v>43858</v>
       </c>
@@ -7058,14 +7065,14 @@
       </c>
       <c r="Q68" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="R68" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>388000</v>
-      </c>
-    </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B69" s="7">
         <v>43859</v>
       </c>
@@ -7108,14 +7115,14 @@
       </c>
       <c r="Q69" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="R69" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>224200</v>
-      </c>
-    </row>
-    <row r="70" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B70" s="7">
         <v>43860</v>
       </c>
@@ -7158,14 +7165,14 @@
       </c>
       <c r="Q70" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="R70" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>434300</v>
-      </c>
-    </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B71" s="7">
         <v>43860</v>
       </c>
@@ -7208,14 +7215,14 @@
       </c>
       <c r="Q71" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="R71" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>331800</v>
-      </c>
-    </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B72" s="7">
         <v>43860</v>
       </c>
@@ -7258,14 +7265,14 @@
       </c>
       <c r="Q72" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="R72" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>406000</v>
-      </c>
-    </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B73" s="7">
         <v>43860</v>
       </c>
@@ -7308,14 +7315,14 @@
       </c>
       <c r="Q73" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="R73" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>442200</v>
-      </c>
-    </row>
-    <row r="74" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B74" s="7">
         <v>43860</v>
       </c>
@@ -7358,14 +7365,14 @@
       </c>
       <c r="Q74" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="R74" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>200600</v>
-      </c>
-    </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B75" s="7">
         <v>43861</v>
       </c>
@@ -7408,14 +7415,14 @@
       </c>
       <c r="Q75" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="R75" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>235600</v>
-      </c>
-    </row>
-    <row r="76" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B76" s="7">
         <v>43861</v>
       </c>
@@ -7458,14 +7465,14 @@
       </c>
       <c r="Q76" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="R76" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>496400</v>
-      </c>
-    </row>
-    <row r="77" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B77" s="7">
         <v>43862</v>
       </c>
@@ -7508,14 +7515,14 @@
       </c>
       <c r="Q77" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="R77" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>313200</v>
-      </c>
-    </row>
-    <row r="78" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B78" s="7">
         <v>43863</v>
       </c>
@@ -7558,14 +7565,14 @@
       </c>
       <c r="Q78" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="R78" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>189000</v>
-      </c>
-    </row>
-    <row r="79" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B79" s="7">
         <v>43864</v>
       </c>
@@ -7608,14 +7615,14 @@
       </c>
       <c r="Q79" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="R79" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>94600</v>
-      </c>
-    </row>
-    <row r="80" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B80" s="7">
         <v>43864</v>
       </c>
@@ -7658,14 +7665,14 @@
       </c>
       <c r="Q80" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="R80" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>637400</v>
-      </c>
-    </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B81" s="7">
         <v>43865</v>
       </c>
@@ -7708,14 +7715,14 @@
       </c>
       <c r="Q81" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="R81" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>827600</v>
-      </c>
-    </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B82" s="7">
         <v>43866</v>
       </c>
@@ -7758,14 +7765,14 @@
       </c>
       <c r="Q82" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>211</v>
+        <v>0</v>
       </c>
       <c r="R82" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>831900</v>
-      </c>
-    </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B83" s="7">
         <v>43866</v>
       </c>
@@ -7808,14 +7815,14 @@
       </c>
       <c r="Q83" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="R83" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>503700</v>
-      </c>
-    </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B84" s="7">
         <v>43867</v>
       </c>
@@ -7858,14 +7865,14 @@
       </c>
       <c r="Q84" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="R84" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>430200</v>
-      </c>
-    </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B85" s="7">
         <v>43867</v>
       </c>
@@ -7908,14 +7915,14 @@
       </c>
       <c r="Q85" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="R85" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>176700</v>
-      </c>
-    </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B86" s="7">
         <v>43868</v>
       </c>
@@ -7958,14 +7965,14 @@
       </c>
       <c r="Q86" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="R86" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>327600</v>
-      </c>
-    </row>
-    <row r="87" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B87" s="7">
         <v>43869</v>
       </c>
@@ -8008,14 +8015,14 @@
       </c>
       <c r="Q87" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="R87" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>724400</v>
-      </c>
-    </row>
-    <row r="88" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B88" s="7">
         <v>43870</v>
       </c>
@@ -8058,14 +8065,14 @@
       </c>
       <c r="Q88" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>153</v>
+        <v>0</v>
       </c>
       <c r="R88" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>566100</v>
-      </c>
-    </row>
-    <row r="89" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B89" s="7">
         <v>43870</v>
       </c>
@@ -8108,14 +8115,14 @@
       </c>
       <c r="Q89" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="R89" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>326600</v>
-      </c>
-    </row>
-    <row r="90" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B90" s="7">
         <v>43871</v>
       </c>
@@ -8158,14 +8165,14 @@
       </c>
       <c r="Q90" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="R90" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>347100</v>
-      </c>
-    </row>
-    <row r="91" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B91" s="7">
         <v>43872</v>
       </c>
@@ -8208,14 +8215,14 @@
       </c>
       <c r="Q91" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="R91" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>406200</v>
-      </c>
-    </row>
-    <row r="92" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B92" s="7">
         <v>43872</v>
       </c>
@@ -8258,14 +8265,14 @@
       </c>
       <c r="Q92" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="R92" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>1368100</v>
-      </c>
-    </row>
-    <row r="93" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B93" s="7">
         <v>43873</v>
       </c>
@@ -8308,14 +8315,14 @@
       </c>
       <c r="Q93" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>302</v>
+        <v>0</v>
       </c>
       <c r="R93" s="16">
         <f t="shared" ca="1" si="7"/>
-        <v>1226500</v>
-      </c>
-    </row>
-    <row r="94" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B94" s="7">
         <v>43874</v>
       </c>
@@ -8358,14 +8365,14 @@
       </c>
       <c r="Q94" s="16">
         <f t="shared" ref="Q94:Q111" ca="1" si="8">SUMIF(I:I,P94,L:L)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="R94" s="16">
         <f t="shared" ref="R94:R111" ca="1" si="9">SUMIF(I:I,P94,N:N)</f>
-        <v>122500</v>
-      </c>
-    </row>
-    <row r="95" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B95" s="7">
         <v>43874</v>
       </c>
@@ -8408,14 +8415,14 @@
       </c>
       <c r="Q95" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="R95" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>94300</v>
-      </c>
-    </row>
-    <row r="96" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B96" s="7">
         <v>43874</v>
       </c>
@@ -8458,14 +8465,14 @@
       </c>
       <c r="Q96" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="R96" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>284700</v>
-      </c>
-    </row>
-    <row r="97" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B97" s="7">
         <v>43874</v>
       </c>
@@ -8508,14 +8515,14 @@
       </c>
       <c r="Q97" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="R97" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>338400</v>
-      </c>
-    </row>
-    <row r="98" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B98" s="7">
         <v>43875</v>
       </c>
@@ -8558,14 +8565,14 @@
       </c>
       <c r="Q98" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="R98" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>475600</v>
-      </c>
-    </row>
-    <row r="99" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B99" s="7">
         <v>43876</v>
       </c>
@@ -8608,14 +8615,14 @@
       </c>
       <c r="Q99" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="R99" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>184000</v>
-      </c>
-    </row>
-    <row r="100" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B100" s="7">
         <v>43876</v>
       </c>
@@ -8658,14 +8665,14 @@
       </c>
       <c r="Q100" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>275</v>
+        <v>0</v>
       </c>
       <c r="R100" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>1143400</v>
-      </c>
-    </row>
-    <row r="101" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B101" s="7">
         <v>43876</v>
       </c>
@@ -8708,14 +8715,14 @@
       </c>
       <c r="Q101" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="R101" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>775600</v>
-      </c>
-    </row>
-    <row r="102" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B102" s="7">
         <v>43877</v>
       </c>
@@ -8758,14 +8765,14 @@
       </c>
       <c r="Q102" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>184</v>
+        <v>0</v>
       </c>
       <c r="R102" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>684900</v>
-      </c>
-    </row>
-    <row r="103" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B103" s="7">
         <v>43878</v>
       </c>
@@ -8808,14 +8815,14 @@
       </c>
       <c r="Q103" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="R103" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>349600</v>
-      </c>
-    </row>
-    <row r="104" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B104" s="7">
         <v>43878</v>
       </c>
@@ -8858,14 +8865,14 @@
       </c>
       <c r="Q104" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="R104" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>327600</v>
-      </c>
-    </row>
-    <row r="105" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B105" s="7">
         <v>43878</v>
       </c>
@@ -8908,14 +8915,14 @@
       </c>
       <c r="Q105" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="R105" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>332500</v>
-      </c>
-    </row>
-    <row r="106" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B106" s="7">
         <v>43878</v>
       </c>
@@ -8958,14 +8965,14 @@
       </c>
       <c r="Q106" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="R106" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>713600</v>
-      </c>
-    </row>
-    <row r="107" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B107" s="7">
         <v>43879</v>
       </c>
@@ -9008,14 +9015,14 @@
       </c>
       <c r="Q107" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="R107" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>619200</v>
-      </c>
-    </row>
-    <row r="108" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B108" s="7">
         <v>43879</v>
       </c>
@@ -9058,14 +9065,14 @@
       </c>
       <c r="Q108" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="R108" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>319600</v>
-      </c>
-    </row>
-    <row r="109" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B109" s="7">
         <v>43880</v>
       </c>
@@ -9108,14 +9115,14 @@
       </c>
       <c r="Q109" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="R109" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>704900</v>
-      </c>
-    </row>
-    <row r="110" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B110" s="7">
         <v>43880</v>
       </c>
@@ -9158,14 +9165,14 @@
       </c>
       <c r="Q110" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>226</v>
+        <v>0</v>
       </c>
       <c r="R110" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>798400</v>
-      </c>
-    </row>
-    <row r="111" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B111" s="7">
         <v>43880</v>
       </c>
@@ -9208,14 +9215,14 @@
       </c>
       <c r="Q111" s="16">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R111" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="112" spans="2:18" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B112" s="7">
         <v>43881</v>
       </c>
@@ -9253,7 +9260,7 @@
         <v>190000</v>
       </c>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B113" s="7">
         <v>43881</v>
       </c>
@@ -9291,7 +9298,7 @@
         <v>53900</v>
       </c>
     </row>
-    <row r="114" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B114" s="7">
         <v>43882</v>
       </c>
@@ -9329,7 +9336,7 @@
         <v>167200</v>
       </c>
     </row>
-    <row r="115" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B115" s="7">
         <v>43883</v>
       </c>
@@ -9367,7 +9374,7 @@
         <v>218400</v>
       </c>
     </row>
-    <row r="116" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="116" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B116" s="7">
         <v>43884</v>
       </c>
@@ -9405,7 +9412,7 @@
         <v>193600</v>
       </c>
     </row>
-    <row r="117" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B117" s="7">
         <v>43885</v>
       </c>
@@ -9443,7 +9450,7 @@
         <v>220900</v>
       </c>
     </row>
-    <row r="118" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="118" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B118" s="7">
         <v>43886</v>
       </c>
@@ -9481,7 +9488,7 @@
         <v>344000</v>
       </c>
     </row>
-    <row r="119" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B119" s="7">
         <v>43886</v>
       </c>
@@ -9519,7 +9526,7 @@
         <v>138600</v>
       </c>
     </row>
-    <row r="120" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B120" s="7">
         <v>43887</v>
       </c>
@@ -9557,7 +9564,7 @@
         <v>38400</v>
       </c>
     </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="121" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B121" s="7">
         <v>43887</v>
       </c>
@@ -9595,7 +9602,7 @@
         <v>87500</v>
       </c>
     </row>
-    <row r="122" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B122" s="7">
         <v>43888</v>
       </c>
@@ -9633,7 +9640,7 @@
         <v>307800</v>
       </c>
     </row>
-    <row r="123" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B123" s="7">
         <v>43888</v>
       </c>
@@ -9671,7 +9678,7 @@
         <v>326600</v>
       </c>
     </row>
-    <row r="124" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B124" s="7">
         <v>43888</v>
       </c>
@@ -9709,7 +9716,7 @@
         <v>162000</v>
       </c>
     </row>
-    <row r="125" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B125" s="7">
         <v>43888</v>
       </c>
@@ -9747,7 +9754,7 @@
         <v>365400</v>
       </c>
     </row>
-    <row r="126" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B126" s="7">
         <v>43888</v>
       </c>
@@ -9785,7 +9792,7 @@
         <v>338200</v>
       </c>
     </row>
-    <row r="127" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="127" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B127" s="7">
         <v>43889</v>
       </c>
@@ -9823,7 +9830,7 @@
         <v>94500</v>
       </c>
     </row>
-    <row r="128" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="128" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B128" s="7">
         <v>43889</v>
       </c>
@@ -9861,7 +9868,7 @@
         <v>171600</v>
       </c>
     </row>
-    <row r="129" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B129" s="7">
         <v>43889</v>
       </c>
@@ -9899,7 +9906,7 @@
         <v>149600</v>
       </c>
     </row>
-    <row r="130" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="130" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B130" s="7">
         <v>43890</v>
       </c>
@@ -9937,7 +9944,7 @@
         <v>107300</v>
       </c>
     </row>
-    <row r="131" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B131" s="7">
         <v>43890</v>
       </c>
@@ -9975,7 +9982,7 @@
         <v>224400</v>
       </c>
     </row>
-    <row r="132" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B132" s="7">
         <v>43890</v>
       </c>
@@ -10013,7 +10020,7 @@
         <v>277200</v>
       </c>
     </row>
-    <row r="133" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B133" s="7">
         <v>43890</v>
       </c>
@@ -10051,7 +10058,7 @@
         <v>273000</v>
       </c>
     </row>
-    <row r="134" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B134" s="7">
         <v>43890</v>
       </c>
@@ -10089,7 +10096,7 @@
         <v>384000</v>
       </c>
     </row>
-    <row r="135" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B135" s="7">
         <v>43890</v>
       </c>
@@ -10127,7 +10134,7 @@
         <v>156000</v>
       </c>
     </row>
-    <row r="136" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B136" s="7">
         <v>43890</v>
       </c>
@@ -10165,7 +10172,7 @@
         <v>350400</v>
       </c>
     </row>
-    <row r="137" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B137" s="7">
         <v>43891</v>
       </c>
@@ -10203,7 +10210,7 @@
         <v>257400</v>
       </c>
     </row>
-    <row r="138" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="138" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B138" s="7">
         <v>43891</v>
       </c>
@@ -10241,7 +10248,7 @@
         <v>356400</v>
       </c>
     </row>
-    <row r="139" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="139" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B139" s="7">
         <v>43891</v>
       </c>
@@ -10279,7 +10286,7 @@
         <v>192400</v>
       </c>
     </row>
-    <row r="140" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B140" s="7">
         <v>43891</v>
       </c>
@@ -10317,7 +10324,7 @@
         <v>229500</v>
       </c>
     </row>
-    <row r="141" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B141" s="7">
         <v>43891</v>
       </c>
@@ -10355,7 +10362,7 @@
         <v>234300</v>
       </c>
     </row>
-    <row r="142" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="142" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B142" s="7">
         <v>43892</v>
       </c>
@@ -10393,7 +10400,7 @@
         <v>153000</v>
       </c>
     </row>
-    <row r="143" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="143" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B143" s="7">
         <v>43892</v>
       </c>
@@ -10431,7 +10438,7 @@
         <v>251100</v>
       </c>
     </row>
-    <row r="144" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="144" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B144" s="7">
         <v>43893</v>
       </c>
@@ -10469,7 +10476,7 @@
         <v>147200</v>
       </c>
     </row>
-    <row r="145" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="145" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B145" s="7">
         <v>43894</v>
       </c>
@@ -10507,7 +10514,7 @@
         <v>352000</v>
       </c>
     </row>
-    <row r="146" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="146" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B146" s="7">
         <v>43895</v>
       </c>
@@ -10545,7 +10552,7 @@
         <v>210700</v>
       </c>
     </row>
-    <row r="147" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="147" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B147" s="7">
         <v>43895</v>
       </c>
@@ -10583,7 +10590,7 @@
         <v>388000</v>
       </c>
     </row>
-    <row r="148" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="148" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B148" s="7">
         <v>43896</v>
       </c>
@@ -10621,7 +10628,7 @@
         <v>224200</v>
       </c>
     </row>
-    <row r="149" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="149" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B149" s="7">
         <v>43897</v>
       </c>
@@ -10659,7 +10666,7 @@
         <v>129000</v>
       </c>
     </row>
-    <row r="150" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="150" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B150" s="7">
         <v>43897</v>
       </c>
@@ -10697,7 +10704,7 @@
         <v>305300</v>
       </c>
     </row>
-    <row r="151" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="151" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B151" s="7">
         <v>43898</v>
       </c>
@@ -10735,7 +10742,7 @@
         <v>331800</v>
       </c>
     </row>
-    <row r="152" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="152" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B152" s="7">
         <v>43898</v>
       </c>
@@ -10773,7 +10780,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="153" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="153" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B153" s="7">
         <v>43898</v>
       </c>
@@ -10811,7 +10818,7 @@
         <v>301000</v>
       </c>
     </row>
-    <row r="154" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="154" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B154" s="7">
         <v>43899</v>
       </c>
@@ -10849,7 +10856,7 @@
         <v>49500</v>
       </c>
     </row>
-    <row r="155" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="155" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B155" s="7">
         <v>43899</v>
       </c>
@@ -10887,7 +10894,7 @@
         <v>117500</v>
       </c>
     </row>
-    <row r="156" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B156" s="7">
         <v>43900</v>
       </c>
@@ -10925,7 +10932,7 @@
         <v>275200</v>
       </c>
     </row>
-    <row r="157" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="157" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B157" s="7">
         <v>43901</v>
       </c>
@@ -10963,7 +10970,7 @@
         <v>130200</v>
       </c>
     </row>
-    <row r="158" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="158" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B158" s="7">
         <v>43901</v>
       </c>
@@ -11001,7 +11008,7 @@
         <v>70400</v>
       </c>
     </row>
-    <row r="159" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="159" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B159" s="7">
         <v>43902</v>
       </c>
@@ -11039,7 +11046,7 @@
         <v>235600</v>
       </c>
     </row>
-    <row r="160" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="160" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B160" s="7">
         <v>43903</v>
       </c>
@@ -11077,7 +11084,7 @@
         <v>89700</v>
       </c>
     </row>
-    <row r="161" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="161" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B161" s="7">
         <v>43904</v>
       </c>
@@ -11115,7 +11122,7 @@
         <v>406700</v>
       </c>
     </row>
-    <row r="162" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="162" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B162" s="7">
         <v>43905</v>
       </c>
@@ -11153,7 +11160,7 @@
         <v>313200</v>
       </c>
     </row>
-    <row r="163" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="163" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B163" s="7">
         <v>43905</v>
       </c>
@@ -11191,7 +11198,7 @@
         <v>189000</v>
       </c>
     </row>
-    <row r="164" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="164" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B164" s="7">
         <v>43905</v>
       </c>
@@ -11229,7 +11236,7 @@
         <v>94600</v>
       </c>
     </row>
-    <row r="165" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="165" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B165" s="7">
         <v>43906</v>
       </c>
@@ -11267,7 +11274,7 @@
         <v>149600</v>
       </c>
     </row>
-    <row r="166" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="166" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B166" s="7">
         <v>43906</v>
       </c>
@@ -11305,7 +11312,7 @@
         <v>105600</v>
       </c>
     </row>
-    <row r="167" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="167" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B167" s="7">
         <v>43906</v>
       </c>
@@ -11343,7 +11350,7 @@
         <v>382200</v>
       </c>
     </row>
-    <row r="168" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="168" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B168" s="7">
         <v>43907</v>
       </c>
@@ -11381,7 +11388,7 @@
         <v>295200</v>
       </c>
     </row>
-    <row r="169" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="169" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B169" s="7">
         <v>43907</v>
       </c>
@@ -11419,7 +11426,7 @@
         <v>308000</v>
       </c>
     </row>
-    <row r="170" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B170" s="7">
         <v>43907</v>
       </c>
@@ -11457,7 +11464,7 @@
         <v>224400</v>
       </c>
     </row>
-    <row r="171" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B171" s="7">
         <v>43908</v>
       </c>
@@ -11495,7 +11502,7 @@
         <v>136000</v>
       </c>
     </row>
-    <row r="172" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="172" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B172" s="7">
         <v>43908</v>
       </c>
@@ -11533,7 +11540,7 @@
         <v>344400</v>
       </c>
     </row>
-    <row r="173" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="173" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B173" s="7">
         <v>43909</v>
       </c>
@@ -11571,7 +11578,7 @@
         <v>351500</v>
       </c>
     </row>
-    <row r="174" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="174" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B174" s="7">
         <v>43909</v>
       </c>
@@ -11609,7 +11616,7 @@
         <v>320100</v>
       </c>
     </row>
-    <row r="175" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="175" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B175" s="7">
         <v>43909</v>
       </c>
@@ -11647,7 +11654,7 @@
         <v>183600</v>
       </c>
     </row>
-    <row r="176" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="176" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B176" s="7">
         <v>43910</v>
       </c>
@@ -11685,7 +11692,7 @@
         <v>88200</v>
       </c>
     </row>
-    <row r="177" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B177" s="7">
         <v>43911</v>
       </c>
@@ -11723,7 +11730,7 @@
         <v>262800</v>
       </c>
     </row>
-    <row r="178" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="178" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B178" s="7">
         <v>43912</v>
       </c>
@@ -11761,7 +11768,7 @@
         <v>79200</v>
       </c>
     </row>
-    <row r="179" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="179" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B179" s="7">
         <v>43912</v>
       </c>
@@ -11799,7 +11806,7 @@
         <v>176700</v>
       </c>
     </row>
-    <row r="180" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B180" s="7">
         <v>43913</v>
       </c>
@@ -11837,7 +11844,7 @@
         <v>327600</v>
       </c>
     </row>
-    <row r="181" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="181" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B181" s="7">
         <v>43913</v>
       </c>
@@ -11875,7 +11882,7 @@
         <v>311600</v>
       </c>
     </row>
-    <row r="182" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B182" s="7">
         <v>43913</v>
       </c>
@@ -11913,7 +11920,7 @@
         <v>412800</v>
       </c>
     </row>
-    <row r="183" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="183" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B183" s="7">
         <v>43914</v>
       </c>
@@ -11951,7 +11958,7 @@
         <v>102400</v>
       </c>
     </row>
-    <row r="184" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B184" s="7">
         <v>43915</v>
       </c>
@@ -11989,7 +11996,7 @@
         <v>247500</v>
       </c>
     </row>
-    <row r="185" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B185" s="7">
         <v>43916</v>
       </c>
@@ -12027,7 +12034,7 @@
         <v>216200</v>
       </c>
     </row>
-    <row r="186" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B186" s="7">
         <v>43916</v>
       </c>
@@ -12065,7 +12072,7 @@
         <v>326600</v>
       </c>
     </row>
-    <row r="187" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="187" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B187" s="7">
         <v>43917</v>
       </c>
@@ -12103,7 +12110,7 @@
         <v>347100</v>
       </c>
     </row>
-    <row r="188" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="188" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B188" s="7">
         <v>43917</v>
       </c>
@@ -12141,7 +12148,7 @@
         <v>112200</v>
       </c>
     </row>
-    <row r="189" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="189" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B189" s="7">
         <v>43917</v>
       </c>
@@ -12179,7 +12186,7 @@
         <v>294000</v>
       </c>
     </row>
-    <row r="190" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="190" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B190" s="7">
         <v>43917</v>
       </c>
@@ -12217,7 +12224,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="191" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="191" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B191" s="7">
         <v>43917</v>
       </c>
@@ -12255,7 +12262,7 @@
         <v>450000</v>
       </c>
     </row>
-    <row r="192" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="192" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B192" s="7">
         <v>43918</v>
       </c>
@@ -12293,7 +12300,7 @@
         <v>366600</v>
       </c>
     </row>
-    <row r="193" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="193" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B193" s="7">
         <v>43918</v>
       </c>
@@ -12331,7 +12338,7 @@
         <v>214500</v>
       </c>
     </row>
-    <row r="194" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="194" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B194" s="7">
         <v>43918</v>
       </c>
@@ -12369,7 +12376,7 @@
         <v>301000</v>
       </c>
     </row>
-    <row r="195" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="195" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B195" s="7">
         <v>43918</v>
       </c>
@@ -12407,7 +12414,7 @@
         <v>225700</v>
       </c>
     </row>
-    <row r="196" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="196" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B196" s="7">
         <v>43918</v>
       </c>
@@ -12445,7 +12452,7 @@
         <v>451200</v>
       </c>
     </row>
-    <row r="197" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="197" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B197" s="7">
         <v>43919</v>
       </c>
@@ -12483,7 +12490,7 @@
         <v>131200</v>
       </c>
     </row>
-    <row r="198" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="198" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B198" s="7">
         <v>43920</v>
       </c>
@@ -12521,7 +12528,7 @@
         <v>106400</v>
       </c>
     </row>
-    <row r="199" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="199" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B199" s="7">
         <v>43921</v>
       </c>
@@ -12559,7 +12566,7 @@
         <v>312000</v>
       </c>
     </row>
-    <row r="200" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="200" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B200" s="7">
         <v>43922</v>
       </c>
@@ -12597,7 +12604,7 @@
         <v>122500</v>
       </c>
     </row>
-    <row r="201" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="201" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B201" s="7">
         <v>43923</v>
       </c>
@@ -12635,7 +12642,7 @@
         <v>94300</v>
       </c>
     </row>
-    <row r="202" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="202" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B202" s="7">
         <v>43923</v>
       </c>
@@ -12673,7 +12680,7 @@
         <v>284700</v>
       </c>
     </row>
-    <row r="203" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="203" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B203" s="7">
         <v>43924</v>
       </c>
@@ -12711,7 +12718,7 @@
         <v>338400</v>
       </c>
     </row>
-    <row r="204" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="204" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B204" s="7">
         <v>43925</v>
       </c>
@@ -12749,7 +12756,7 @@
         <v>333000</v>
       </c>
     </row>
-    <row r="205" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="205" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B205" s="7">
         <v>43925</v>
       </c>
@@ -12787,7 +12794,7 @@
         <v>142600</v>
       </c>
     </row>
-    <row r="206" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="206" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B206" s="7">
         <v>43925</v>
       </c>
@@ -12825,7 +12832,7 @@
         <v>184000</v>
       </c>
     </row>
-    <row r="207" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="207" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B207" s="7">
         <v>43925</v>
       </c>
@@ -12863,7 +12870,7 @@
         <v>332500</v>
       </c>
     </row>
-    <row r="208" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="208" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B208" s="7">
         <v>43926</v>
       </c>
@@ -12901,7 +12908,7 @@
         <v>41000</v>
       </c>
     </row>
-    <row r="209" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="209" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B209" s="7">
         <v>43926</v>
       </c>
@@ -12939,7 +12946,7 @@
         <v>405000</v>
       </c>
     </row>
-    <row r="210" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="210" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B210" s="7">
         <v>43926</v>
       </c>
@@ -12977,7 +12984,7 @@
         <v>364900</v>
       </c>
     </row>
-    <row r="211" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="211" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B211" s="7">
         <v>43927</v>
       </c>
@@ -13015,7 +13022,7 @@
         <v>369600</v>
       </c>
     </row>
-    <row r="212" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="212" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B212" s="7">
         <v>43927</v>
       </c>
@@ -13053,7 +13060,7 @@
         <v>220000</v>
       </c>
     </row>
-    <row r="213" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="213" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B213" s="7">
         <v>43927</v>
       </c>
@@ -13091,7 +13098,7 @@
         <v>186000</v>
       </c>
     </row>
-    <row r="214" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="214" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B214" s="7">
         <v>43927</v>
       </c>
@@ -13129,7 +13136,7 @@
         <v>195000</v>
       </c>
     </row>
-    <row r="215" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="215" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B215" s="7">
         <v>43928</v>
       </c>
@@ -13167,7 +13174,7 @@
         <v>75600</v>
       </c>
     </row>
-    <row r="216" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="216" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B216" s="7">
         <v>43929</v>
       </c>
@@ -13205,7 +13212,7 @@
         <v>285600</v>
       </c>
     </row>
-    <row r="217" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="217" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B217" s="7">
         <v>43930</v>
       </c>
@@ -13243,7 +13250,7 @@
         <v>128700</v>
       </c>
     </row>
-    <row r="218" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="218" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B218" s="7">
         <v>43931</v>
       </c>
@@ -13281,7 +13288,7 @@
         <v>349600</v>
       </c>
     </row>
-    <row r="219" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="219" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B219" s="7">
         <v>43931</v>
       </c>
@@ -13319,7 +13326,7 @@
         <v>327600</v>
       </c>
     </row>
-    <row r="220" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="220" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B220" s="7">
         <v>43931</v>
       </c>
@@ -13357,7 +13364,7 @@
         <v>332500</v>
       </c>
     </row>
-    <row r="221" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="221" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B221" s="7">
         <v>43932</v>
       </c>
@@ -13395,7 +13402,7 @@
         <v>475200</v>
       </c>
     </row>
-    <row r="222" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="222" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B222" s="7">
         <v>43932</v>
       </c>
@@ -13433,7 +13440,7 @@
         <v>70400</v>
       </c>
     </row>
-    <row r="223" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="223" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B223" s="7">
         <v>43933</v>
       </c>
@@ -13471,7 +13478,7 @@
         <v>168000</v>
       </c>
     </row>
-    <row r="224" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="224" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B224" s="7">
         <v>43934</v>
       </c>
@@ -13509,7 +13516,7 @@
         <v>455400</v>
       </c>
     </row>
-    <row r="225" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="225" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B225" s="7">
         <v>43934</v>
       </c>
@@ -13547,7 +13554,7 @@
         <v>163800</v>
       </c>
     </row>
-    <row r="226" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="226" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B226" s="7">
         <v>43934</v>
       </c>
@@ -13585,7 +13592,7 @@
         <v>319600</v>
       </c>
     </row>
-    <row r="227" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="227" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B227" s="7">
         <v>43935</v>
       </c>
@@ -13623,7 +13630,7 @@
         <v>207000</v>
       </c>
     </row>
-    <row r="228" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="228" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B228" s="7">
         <v>43935</v>
       </c>
@@ -13661,7 +13668,7 @@
         <v>254100</v>
       </c>
     </row>
-    <row r="229" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="229" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B229" s="7">
         <v>43935</v>
       </c>
@@ -13699,7 +13706,7 @@
         <v>243800</v>
       </c>
     </row>
-    <row r="230" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="230" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B230" s="7">
         <v>43936</v>
       </c>
@@ -13737,7 +13744,7 @@
         <v>297000</v>
       </c>
     </row>
-    <row r="231" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="231" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I231" s="21">
         <v>43935</v>
       </c>
@@ -13757,7 +13764,7 @@
         <v>197200</v>
       </c>
     </row>
-    <row r="232" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="232" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I232" s="21">
         <v>43935</v>
       </c>
@@ -13777,7 +13784,7 @@
         <v>304200</v>
       </c>
     </row>
-    <row r="233" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="233" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I233" s="21">
         <v>43936</v>
       </c>

</xml_diff>